<commit_message>
Cleanup: Removed unnecessary Python files and duplicate data
</commit_message>
<xml_diff>
--- a/lighthouse_scores_summary.xlsx
+++ b/lighthouse_scores_summary.xlsx
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -714,7 +714,7 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -794,7 +794,7 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -874,7 +874,7 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -914,7 +914,7 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -954,7 +954,7 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -986,7 +986,7 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="J15" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -1066,7 +1066,7 @@
         </is>
       </c>
       <c r="J16" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -1106,7 +1106,7 @@
         </is>
       </c>
       <c r="J17" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -1146,7 +1146,7 @@
         </is>
       </c>
       <c r="J18" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -1186,7 +1186,7 @@
         </is>
       </c>
       <c r="J19" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1226,7 +1226,7 @@
         </is>
       </c>
       <c r="J20" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -1266,7 +1266,7 @@
         </is>
       </c>
       <c r="J21" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
@@ -1306,7 +1306,7 @@
         </is>
       </c>
       <c r="J22" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -1346,7 +1346,7 @@
         </is>
       </c>
       <c r="J23" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
@@ -1386,7 +1386,7 @@
         </is>
       </c>
       <c r="J24" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
@@ -1418,7 +1418,7 @@
         </is>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
@@ -1458,7 +1458,7 @@
         </is>
       </c>
       <c r="J26" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
@@ -1498,7 +1498,7 @@
         </is>
       </c>
       <c r="J27" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1538,7 +1538,7 @@
         </is>
       </c>
       <c r="J28" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -1578,7 +1578,7 @@
         </is>
       </c>
       <c r="J29" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
@@ -1618,7 +1618,7 @@
         </is>
       </c>
       <c r="J30" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
@@ -1658,7 +1658,7 @@
         </is>
       </c>
       <c r="J31" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
@@ -1730,7 +1730,7 @@
         </is>
       </c>
       <c r="J33" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
@@ -1770,7 +1770,7 @@
         </is>
       </c>
       <c r="J34" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35">
@@ -1810,7 +1810,7 @@
         </is>
       </c>
       <c r="J35" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1850,7 +1850,7 @@
         </is>
       </c>
       <c r="J36" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="J37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1922,7 +1922,7 @@
         </is>
       </c>
       <c r="J38" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -1954,7 +1954,7 @@
         </is>
       </c>
       <c r="J39" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40">
@@ -1994,7 +1994,7 @@
         </is>
       </c>
       <c r="J40" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41">
@@ -2034,7 +2034,7 @@
         </is>
       </c>
       <c r="J41" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
@@ -2074,7 +2074,7 @@
         </is>
       </c>
       <c r="J42" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
@@ -2114,7 +2114,7 @@
         </is>
       </c>
       <c r="J43" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44">
@@ -2154,7 +2154,7 @@
         </is>
       </c>
       <c r="J44" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45">
@@ -2194,7 +2194,7 @@
         </is>
       </c>
       <c r="J45" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
@@ -2234,7 +2234,7 @@
         </is>
       </c>
       <c r="J46" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
@@ -2274,7 +2274,7 @@
         </is>
       </c>
       <c r="J47" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
@@ -2314,7 +2314,7 @@
         </is>
       </c>
       <c r="J48" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -2354,7 +2354,7 @@
         </is>
       </c>
       <c r="J49" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
@@ -2394,7 +2394,7 @@
         </is>
       </c>
       <c r="J50" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51">
@@ -2474,7 +2474,7 @@
         </is>
       </c>
       <c r="J52" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53">
@@ -2514,7 +2514,7 @@
         </is>
       </c>
       <c r="J53" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
@@ -2554,7 +2554,7 @@
         </is>
       </c>
       <c r="J54" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55">
@@ -2594,7 +2594,7 @@
         </is>
       </c>
       <c r="J55" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56">
@@ -2634,7 +2634,7 @@
         </is>
       </c>
       <c r="J56" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57">
@@ -2674,7 +2674,7 @@
         </is>
       </c>
       <c r="J57" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
@@ -2714,7 +2714,7 @@
         </is>
       </c>
       <c r="J58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59">
@@ -2754,7 +2754,7 @@
         </is>
       </c>
       <c r="J59" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -2794,7 +2794,7 @@
         </is>
       </c>
       <c r="J60" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61">
@@ -2834,7 +2834,7 @@
         </is>
       </c>
       <c r="J61" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
@@ -2874,7 +2874,7 @@
         </is>
       </c>
       <c r="J62" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63">
@@ -2914,7 +2914,7 @@
         </is>
       </c>
       <c r="J63" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64">
@@ -2954,7 +2954,7 @@
         </is>
       </c>
       <c r="J64" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65">
@@ -2994,7 +2994,7 @@
         </is>
       </c>
       <c r="J65" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66">
@@ -3034,7 +3034,7 @@
         </is>
       </c>
       <c r="J66" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67">
@@ -3074,7 +3074,7 @@
         </is>
       </c>
       <c r="J67" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -3114,7 +3114,7 @@
         </is>
       </c>
       <c r="J68" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -3154,7 +3154,7 @@
         </is>
       </c>
       <c r="J69" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
@@ -3194,7 +3194,7 @@
         </is>
       </c>
       <c r="J70" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -3234,7 +3234,7 @@
         </is>
       </c>
       <c r="J71" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -3274,7 +3274,7 @@
         </is>
       </c>
       <c r="J72" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -3314,7 +3314,7 @@
         </is>
       </c>
       <c r="J73" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74">
@@ -3354,7 +3354,7 @@
         </is>
       </c>
       <c r="J74" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
@@ -3394,7 +3394,7 @@
         </is>
       </c>
       <c r="J75" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76">
@@ -3434,7 +3434,7 @@
         </is>
       </c>
       <c r="J76" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -3474,7 +3474,7 @@
         </is>
       </c>
       <c r="J77" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78">
@@ -3514,7 +3514,7 @@
         </is>
       </c>
       <c r="J78" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79">
@@ -3554,7 +3554,7 @@
         </is>
       </c>
       <c r="J79" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -3594,7 +3594,7 @@
         </is>
       </c>
       <c r="J80" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81">
@@ -3634,7 +3634,7 @@
         </is>
       </c>
       <c r="J81" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -3674,7 +3674,7 @@
         </is>
       </c>
       <c r="J82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83">
@@ -3714,7 +3714,7 @@
         </is>
       </c>
       <c r="J83" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84">
@@ -3754,7 +3754,7 @@
         </is>
       </c>
       <c r="J84" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85">
@@ -3794,7 +3794,7 @@
         </is>
       </c>
       <c r="J85" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86">
@@ -3834,7 +3834,7 @@
         </is>
       </c>
       <c r="J86" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87">
@@ -3874,7 +3874,7 @@
         </is>
       </c>
       <c r="J87" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88">
@@ -3914,7 +3914,7 @@
         </is>
       </c>
       <c r="J88" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -3954,7 +3954,7 @@
         </is>
       </c>
       <c r="J89" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90">
@@ -3994,7 +3994,7 @@
         </is>
       </c>
       <c r="J90" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91">
@@ -4026,7 +4026,7 @@
         </is>
       </c>
       <c r="J91" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92">
@@ -4066,7 +4066,7 @@
         </is>
       </c>
       <c r="J92" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
@@ -4106,7 +4106,7 @@
         </is>
       </c>
       <c r="J93" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94">
@@ -4146,7 +4146,7 @@
         </is>
       </c>
       <c r="J94" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95">
@@ -4186,7 +4186,7 @@
         </is>
       </c>
       <c r="J95" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -4226,7 +4226,7 @@
         </is>
       </c>
       <c r="J96" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97">
@@ -4266,7 +4266,7 @@
         </is>
       </c>
       <c r="J97" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98">
@@ -4306,7 +4306,7 @@
         </is>
       </c>
       <c r="J98" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99">
@@ -4346,7 +4346,7 @@
         </is>
       </c>
       <c r="J99" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -4386,7 +4386,7 @@
         </is>
       </c>
       <c r="J100" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>